<commit_message>
Se actualiza la llamada de los datos de prueba del proyecto.Invocacion via DataDriver
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Data.xlsx
+++ b/src/test/resources/data/Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domingo.saavedra\Downloads\DemoFrameworkBootCamp\src\test\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodolfo.cancino\Desktop\DemoFrameworkBootCamp\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E363A206-CD75-40F6-85A3-5A30E7C27F3B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B9E492-F7CF-4B7D-B574-689D862A187F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10404" xr2:uid="{E6394DFB-6163-4A1C-B561-81F0B75BD956}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10400" xr2:uid="{E6394DFB-6163-4A1C-B561-81F0B75BD956}"/>
   </bookViews>
   <sheets>
     <sheet name="DataPruebas" sheetId="1" r:id="rId1"/>
@@ -608,16 +608,16 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -652,7 +652,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
@@ -683,7 +683,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>56</v>
       </c>
@@ -714,7 +714,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -737,7 +737,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -756,7 +756,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -783,7 +783,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -806,7 +806,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -825,7 +825,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -848,7 +848,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -863,7 +863,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -878,7 +878,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -893,7 +893,7 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -908,7 +908,7 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -923,7 +923,7 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -938,7 +938,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -953,7 +953,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -968,7 +968,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -983,7 +983,7 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -998,7 +998,7 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -1029,7 +1029,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1043,12 +1043,12 @@
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>47</v>
       </c>
@@ -1104,7 +1104,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1129,7 +1129,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1146,7 +1146,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1177,7 +1177,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1208,7 +1208,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1229,7 +1229,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1244,7 +1244,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>48</v>
       </c>
@@ -1259,7 +1259,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -1274,7 +1274,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -1289,7 +1289,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -1304,7 +1304,7 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -1319,7 +1319,7 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -1334,7 +1334,7 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -1349,7 +1349,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -1364,7 +1364,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -1379,7 +1379,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -1394,7 +1394,7 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -1409,7 +1409,7 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -1435,7 +1435,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1447,7 +1447,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1459,7 +1459,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1471,7 +1471,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1483,7 +1483,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1495,7 +1495,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1507,7 +1507,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>